<commit_message>
my account page excuted for ios and android
</commit_message>
<xml_diff>
--- a/apps/features/backlog/iPhone/get_support.xlsx
+++ b/apps/features/backlog/iPhone/get_support.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\iPhone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\iPhone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275DAB00-39FA-4E3C-B321-4C52721467BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CA090E-9BFA-424E-BAC5-D403256624AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1185,8 +1185,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1341,7 +1341,7 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>15</v>
       </c>

</xml_diff>